<commit_message>
atualização que o Alexandre  pediu
</commit_message>
<xml_diff>
--- a/Plan_Contas_AP_ADIANTAMENTO_HEADER_20220331_GOLIVE.xlsx
+++ b/Plan_Contas_AP_ADIANTAMENTO_HEADER_20220331_GOLIVE.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW114"/>
+  <dimension ref="A1:CW110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +442,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>172253.24</t>
+          <t>75070.11</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -626,17 +626,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ADTO_MERLIVRE CANCELA</t>
+          <t>ADTO_SINDICOMERCIOMAR</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>24.83</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-04-08</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-04-08</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
@@ -815,28 +815,28 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ADTO_PONTE ROLANTE</t>
+          <t>ADTO_SINDICATO032022</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>120.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2021-10-04</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>483</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>483</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>2021-10-04</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="V3" t="inlineStr"/>
@@ -1004,28 +1004,28 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ADTO_09032022</t>
+          <t>ADTO_SINDIMETAL 03202</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>755.34</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2022-03-09</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>628</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>628</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>2022-03-09</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="V4" t="inlineStr"/>
@@ -1193,28 +1193,28 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ADTO_01042022</t>
+          <t>ADTO_SINDIMETAL032022</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>41.75</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2022-04-01</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>628</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>628</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>2022-04-01</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="V5" t="inlineStr"/>
@@ -1382,28 +1382,28 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ADTO_22062021</t>
+          <t>ADTO_SINDIMETAL 03202</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1326.01</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2021-06-22</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1625</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1625</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>2021-06-22</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="V6" t="inlineStr"/>
@@ -1571,28 +1571,28 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ADTO_2206958</t>
+          <t>ADTO_PONTE ROLANTE</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>145200.00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2021-10-04</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2669</t>
+          <t>483</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2669</t>
+          <t>483</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2021-10-04</t>
         </is>
       </c>
       <c r="V7" t="inlineStr"/>
@@ -1760,28 +1760,28 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ADTO_10022022 1PARC</t>
+          <t>ADTO_PONTE ROLANTE</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>338800.00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2022-02-10</t>
+          <t>2022-04-07</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>11085</t>
+          <t>483</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>11085</t>
+          <t>483</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>2022-02-10</t>
+          <t>2022-04-07</t>
         </is>
       </c>
       <c r="V8" t="inlineStr"/>
@@ -1949,28 +1949,28 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ADTO_10032022</t>
+          <t>ADTO_09032022</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>13112.92</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-09</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>11085</t>
+          <t>628</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>11085</t>
+          <t>628</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-09</t>
         </is>
       </c>
       <c r="V9" t="inlineStr"/>
@@ -2138,28 +2138,28 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ADTO_1660936</t>
+          <t>ADTO_01042022</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.78</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2010-05-06</t>
+          <t>2022-04-01</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>14806</t>
+          <t>628</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>14806</t>
+          <t>628</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -2195,7 +2195,7 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>2010-05-06</t>
+          <t>2022-04-01</t>
         </is>
       </c>
       <c r="V10" t="inlineStr"/>
@@ -2327,28 +2327,28 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ADTO_6882020135050461</t>
+          <t>ADTO_22062021</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>8991.53</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2013-11-04</t>
+          <t>2021-06-22</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>26340</t>
+          <t>1625</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>26340</t>
+          <t>1625</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>2013-11-04</t>
+          <t>2021-06-22</t>
         </is>
       </c>
       <c r="V11" t="inlineStr"/>
@@ -2516,28 +2516,28 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ADTO_1065672011505003</t>
+          <t>ADTO_10022022 1PARC</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>3206.86</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2013-11-04</t>
+          <t>2022-02-10</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>26340</t>
+          <t>11085</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>26340</t>
+          <t>11085</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>2013-11-04</t>
+          <t>2022-02-10</t>
         </is>
       </c>
       <c r="V12" t="inlineStr"/>
@@ -2705,28 +2705,28 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ADTO_1049282013505046</t>
+          <t>ADTO_10032022</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>3206.86</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2014-11-20</t>
+          <t>2022-03-10</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>26340</t>
+          <t>11085</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>26340</t>
+          <t>11085</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>2014-11-20</t>
+          <t>2022-03-10</t>
         </is>
       </c>
       <c r="V13" t="inlineStr"/>
@@ -2894,28 +2894,28 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ADTO_6882020135050461</t>
+          <t>ADTO_11042022</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>3206.86</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2013-11-01</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>26341</t>
+          <t>11085</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>26341</t>
+          <t>11085</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>2013-11-01</t>
+          <t>2022-04-11</t>
         </is>
       </c>
       <c r="V14" t="inlineStr"/>
@@ -3083,28 +3083,28 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ADTO_TX 4,65 NF 21552</t>
+          <t>ADTO_1660936</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>10177.31</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022-02-18</t>
+          <t>2010-05-06</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>26341</t>
+          <t>14806</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>26341</t>
+          <t>14806</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -3140,7 +3140,7 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>2022-02-18</t>
+          <t>2010-05-06</t>
         </is>
       </c>
       <c r="V15" t="inlineStr"/>
@@ -3272,28 +3272,28 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ADTO_18032022</t>
+          <t>ADTO_6882020135050461</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>7058.11</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022-03-18</t>
+          <t>2013-11-04</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>27783</t>
+          <t>26340</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>27783</t>
+          <t>26340</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>2022-03-18</t>
+          <t>2013-11-04</t>
         </is>
       </c>
       <c r="V16" t="inlineStr"/>
@@ -3461,28 +3461,28 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM MARCO2022</t>
+          <t>ADTO_1065672011505003</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>4200.00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-03-16</t>
+          <t>2013-11-04</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>28042</t>
+          <t>26340</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>28042</t>
+          <t>26340</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>2022-03-16</t>
+          <t>2013-11-04</t>
         </is>
       </c>
       <c r="V17" t="inlineStr"/>
@@ -3650,28 +3650,28 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM ABRIL2022</t>
+          <t>ADTO_1049282013505046</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>7485.83</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2014-11-20</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>31027</t>
+          <t>26340</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>31027</t>
+          <t>26340</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -3707,7 +3707,7 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2014-11-20</t>
         </is>
       </c>
       <c r="V18" t="inlineStr"/>
@@ -3839,28 +3839,28 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ADTO_2114565720</t>
+          <t>ADTO_6882020135050461</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>400.00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2013-11-01</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>32213</t>
+          <t>26341</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>32213</t>
+          <t>26341</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2013-11-01</t>
         </is>
       </c>
       <c r="V19" t="inlineStr"/>
@@ -4028,28 +4028,28 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTOS</t>
+          <t>ADTO_6389 VACINAS</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>21183.76</t>
+          <t>3000.00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2018-12-31</t>
+          <t>2022-04-08</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>32238</t>
+          <t>26345</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>32238</t>
+          <t>26345</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>2018-12-31</t>
+          <t>2022-04-08</t>
         </is>
       </c>
       <c r="V20" t="inlineStr"/>
@@ -4217,28 +4217,28 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTOS.</t>
+          <t>ADTO_VIAGEM ABRIL2022</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>15692.10</t>
+          <t>2500.00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2018-12-31</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>32238</t>
+          <t>31027</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>32238</t>
+          <t>31027</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -4274,7 +4274,7 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>2018-12-31</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="V21" t="inlineStr"/>
@@ -4406,12 +4406,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTO</t>
+          <t>ADTO_PAGAMENTOS</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2885.12</t>
+          <t>10591.88</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -4595,12 +4595,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTOS072018</t>
+          <t>ADTO_PAGAMENTOS.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1521.72</t>
+          <t>46432.80</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -4784,12 +4784,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTOS0818</t>
+          <t>ADTO_PAGAMENTO</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1109.86</t>
+          <t>1442.56</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -4973,12 +4973,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTOS0918</t>
+          <t>ADTO_PAGAMENTOS072018</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1429.44</t>
+          <t>760.86</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -5162,12 +5162,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTOS1018</t>
+          <t>ADTO_PAGAMENTOS0818</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1312.00</t>
+          <t>554.93</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -5351,12 +5351,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ADTO_PAGAMENTOS1218</t>
+          <t>ADTO_PAGAMENTOS0918</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>256.00</t>
+          <t>714.72</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -5540,28 +5540,28 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ADTO_1005-2 TIO</t>
+          <t>ADTO_PAGAMENTOS1018</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>656.00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2010-11-30</t>
+          <t>2018-12-31</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>32437</t>
+          <t>32238</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>32437</t>
+          <t>32238</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -5597,7 +5597,7 @@
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>2010-11-30</t>
+          <t>2018-12-31</t>
         </is>
       </c>
       <c r="V28" t="inlineStr"/>
@@ -5729,28 +5729,28 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ADTO_650</t>
+          <t>ADTO_PAGAMENTOS1218</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>128.00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2009-05-19</t>
+          <t>2018-12-31</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>33285</t>
+          <t>32238</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>33285</t>
+          <t>32238</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -5786,7 +5786,7 @@
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>2009-05-19</t>
+          <t>2018-12-31</t>
         </is>
       </c>
       <c r="V29" t="inlineStr"/>
@@ -5918,28 +5918,28 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ADTO_GW1-11120A01-01</t>
+          <t>ADTO_1005-2 TIO</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>118.00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2012-04-26</t>
+          <t>2010-11-30</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>33823</t>
+          <t>32437</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>33823</t>
+          <t>32437</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -5975,7 +5975,7 @@
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>2012-04-26</t>
+          <t>2010-11-30</t>
         </is>
       </c>
       <c r="V30" t="inlineStr"/>
@@ -6107,28 +6107,28 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ADTO_59000198011</t>
+          <t>ADTO_650</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>531772.00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2013-07-05</t>
+          <t>2009-05-19</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>33823</t>
+          <t>33285</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
         <is>
-          <t>33823</t>
+          <t>33285</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -6164,7 +6164,7 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>2013-07-05</t>
+          <t>2009-05-19</t>
         </is>
       </c>
       <c r="V31" t="inlineStr"/>
@@ -6296,17 +6296,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>ADTO_001-CMM ITALIA</t>
+          <t>ADTO_GW1-11120A01-01</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>14907.56</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2014-05-27</t>
+          <t>2012-04-26</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -6353,7 +6353,7 @@
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>2014-05-27</t>
+          <t>2012-04-26</t>
         </is>
       </c>
       <c r="V32" t="inlineStr"/>
@@ -6485,17 +6485,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ADTO_SGW-4312-01 HYUN</t>
+          <t>ADTO_59000198011</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>21.20</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2014-08-05</t>
+          <t>2013-07-05</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>2014-08-05</t>
+          <t>2013-07-05</t>
         </is>
       </c>
       <c r="V33" t="inlineStr"/>
@@ -6674,28 +6674,28 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ADTO_GW1-11120A01-01</t>
+          <t>ADTO_001-CMM ITALIA</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>3879.61</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2012-04-27</t>
+          <t>2014-05-27</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>35977</t>
+          <t>33823</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
-          <t>35977</t>
+          <t>33823</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -6731,7 +6731,7 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>2012-04-27</t>
+          <t>2014-05-27</t>
         </is>
       </c>
       <c r="V34" t="inlineStr"/>
@@ -6863,28 +6863,28 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ADTO_GW1-120117A-01</t>
+          <t>ADTO_SGW-4312-01 HYUN</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>99731.03</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2012-04-27</t>
+          <t>2014-08-05</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>35977</t>
+          <t>33823</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr">
         <is>
-          <t>35977</t>
+          <t>33823</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -6920,7 +6920,7 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>2012-04-27</t>
+          <t>2014-08-05</t>
         </is>
       </c>
       <c r="V35" t="inlineStr"/>
@@ -7052,28 +7052,28 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ADTO_590-6801</t>
+          <t>ADTO_GW1-11120A01-01</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>280.00</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2011-05-16</t>
+          <t>2012-04-27</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>36683</t>
+          <t>35977</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
-          <t>36683</t>
+          <t>35977</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -7109,7 +7109,7 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>2011-05-16</t>
+          <t>2012-04-27</t>
         </is>
       </c>
       <c r="V36" t="inlineStr"/>
@@ -7241,28 +7241,28 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ADTO_590-5540</t>
+          <t>ADTO_GW1-120117A-01</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>280.00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2010-10-07</t>
+          <t>2012-04-27</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>36687</t>
+          <t>35977</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>36687</t>
+          <t>35977</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -7298,7 +7298,7 @@
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>2010-10-07</t>
+          <t>2012-04-27</t>
         </is>
       </c>
       <c r="V37" t="inlineStr"/>
@@ -7430,28 +7430,28 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ADTO_1005-TIONA</t>
+          <t>ADTO_590-6801</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>6983.23</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2010-11-05</t>
+          <t>2011-05-16</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>36687</t>
+          <t>36683</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr">
         <is>
-          <t>36687</t>
+          <t>36683</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -7487,7 +7487,7 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>2010-11-05</t>
+          <t>2011-05-16</t>
         </is>
       </c>
       <c r="V38" t="inlineStr"/>
@@ -7619,17 +7619,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ADTO_5900013001</t>
+          <t>ADTO_590-5540</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>16535.00</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2012-02-23</t>
+          <t>2010-10-07</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -7676,7 +7676,7 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>2012-02-23</t>
+          <t>2010-10-07</t>
         </is>
       </c>
       <c r="V39" t="inlineStr"/>
@@ -7808,17 +7808,17 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ADTO_5900013001</t>
+          <t>ADTO_1005-TIONA</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2775.00</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2012-03-14</t>
+          <t>2010-11-05</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -7865,7 +7865,7 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>2012-03-14</t>
+          <t>2010-11-05</t>
         </is>
       </c>
       <c r="V40" t="inlineStr"/>
@@ -7997,28 +7997,28 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ADTO_1005-2 TIO</t>
+          <t>ADTO_5900013001</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>20.28</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2010-12-20</t>
+          <t>2012-02-23</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>37428</t>
+          <t>36687</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
-          <t>37428</t>
+          <t>36687</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -8054,7 +8054,7 @@
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>2010-12-20</t>
+          <t>2012-02-23</t>
         </is>
       </c>
       <c r="V41" t="inlineStr"/>
@@ -8186,28 +8186,28 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ADTO_28122020CARTAO</t>
+          <t>ADTO_5900013001</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>5.25</t>
+          <t>439.20</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2021-02-10</t>
+          <t>2012-03-14</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>43352</t>
+          <t>36687</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
-          <t>43352</t>
+          <t>36687</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -8243,7 +8243,7 @@
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>2021-02-10</t>
+          <t>2012-03-14</t>
         </is>
       </c>
       <c r="V42" t="inlineStr"/>
@@ -8375,28 +8375,28 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ADTO_TDB 002</t>
+          <t>ADTO_1005-2 TIO</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>478.50</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2012-11-23</t>
+          <t>2010-12-20</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>45966</t>
+          <t>37428</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr">
         <is>
-          <t>45966</t>
+          <t>37428</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -8432,7 +8432,7 @@
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>2012-11-23</t>
+          <t>2010-12-20</t>
         </is>
       </c>
       <c r="V43" t="inlineStr"/>
@@ -8564,28 +8564,28 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ADTO_TDB 002</t>
+          <t>ADTO_28122020CARTAO</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>35.06</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2012-11-27</t>
+          <t>2021-02-10</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>45966</t>
+          <t>43352</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr">
         <is>
-          <t>45966</t>
+          <t>43352</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -8621,7 +8621,7 @@
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>2012-11-27</t>
+          <t>2021-02-10</t>
         </is>
       </c>
       <c r="V44" t="inlineStr"/>
@@ -8758,23 +8758,23 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>376.73</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2012-12-18</t>
+          <t>2012-11-23</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>46219</t>
+          <t>45966</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr">
         <is>
-          <t>46219</t>
+          <t>45966</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -8810,7 +8810,7 @@
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>2012-12-18</t>
+          <t>2012-11-23</t>
         </is>
       </c>
       <c r="V45" t="inlineStr"/>
@@ -8942,28 +8942,28 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>ADTO_INFRACAO CLIENTE</t>
+          <t>ADTO_TDB 002</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>440.71</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2020-10-02</t>
+          <t>2012-11-27</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>47493</t>
+          <t>45966</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr">
         <is>
-          <t>47493</t>
+          <t>45966</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -8999,7 +8999,7 @@
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>2020-10-02</t>
+          <t>2012-11-27</t>
         </is>
       </c>
       <c r="V46" t="inlineStr"/>
@@ -9131,28 +9131,28 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ADTO_ANT. ALUGUEIS</t>
+          <t>ADTO_TDB 002</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>264.36</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2021-07-05</t>
+          <t>2012-12-18</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>48910</t>
+          <t>46219</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>48910</t>
+          <t>46219</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>2021-07-05</t>
+          <t>2012-12-18</t>
         </is>
       </c>
       <c r="V47" t="inlineStr"/>
@@ -9320,28 +9320,28 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ADTO_25032022</t>
+          <t>ADTO_INFRACAO CLIENTE</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>7222.30</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2020-10-02</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>53850</t>
+          <t>47493</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr">
         <is>
-          <t>53850</t>
+          <t>47493</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -9377,7 +9377,7 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2020-10-02</t>
         </is>
       </c>
       <c r="V48" t="inlineStr"/>
@@ -9509,28 +9509,28 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM ABRIL2022</t>
+          <t>ADTO_ANT. ALUGUEIS</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>10000.00</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2021-07-05</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>54568</t>
+          <t>48910</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
-          <t>54568</t>
+          <t>48910</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -9566,7 +9566,7 @@
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2021-07-05</t>
         </is>
       </c>
       <c r="V49" t="inlineStr"/>
@@ -9698,28 +9698,28 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>ADTO_CARTAO08022022</t>
+          <t>ADTO_VIAGEM ABRIL2022</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1800.00</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>61840</t>
+          <t>54568</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr">
         <is>
-          <t>61840</t>
+          <t>54568</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="V50" t="inlineStr"/>
@@ -9892,7 +9892,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>7512.00</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -10081,7 +10081,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2304.00</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -10270,7 +10270,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>720.00</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -10459,7 +10459,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1752.00</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -10648,7 +10648,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>13128.00</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -10837,7 +10837,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>864.00</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -11026,7 +11026,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1440.00</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -11215,7 +11215,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>3192.00</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -11404,7 +11404,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>34250.00</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -11593,7 +11593,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>17750.00</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -11782,7 +11782,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2500.00</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -11966,28 +11966,28 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>ADTO_30032022</t>
+          <t>ADTO_VIAGEM ABRIL2022</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2500.00</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>70630</t>
+          <t>71358</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr">
         <is>
-          <t>70630</t>
+          <t>71358</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -12023,7 +12023,7 @@
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="V62" t="inlineStr"/>
@@ -12155,28 +12155,28 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM ABRIL2022</t>
+          <t>ADTO_CAUCAOALUGUEL</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>6000.00</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2018-07-24</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>71358</t>
+          <t>76631</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
         <is>
-          <t>71358</t>
+          <t>76631</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -12212,7 +12212,7 @@
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2018-07-24</t>
         </is>
       </c>
       <c r="V63" t="inlineStr"/>
@@ -12344,28 +12344,28 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>ADTO_CAUCAOALUGUEL</t>
+          <t>ADTO_14122021</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1857.39</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2018-07-24</t>
+          <t>2021-12-14</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>76631</t>
+          <t>76912</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr">
         <is>
-          <t>76631</t>
+          <t>76912</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -12401,7 +12401,7 @@
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>2018-07-24</t>
+          <t>2021-12-14</t>
         </is>
       </c>
       <c r="V64" t="inlineStr"/>
@@ -12533,17 +12533,17 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>ADTO_14122021</t>
+          <t>ADTO_DIVCT 10012022</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>245.00</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2021-12-14</t>
+          <t>2022-01-10</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -12590,7 +12590,7 @@
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>2021-12-14</t>
+          <t>2022-01-10</t>
         </is>
       </c>
       <c r="V65" t="inlineStr"/>
@@ -12722,17 +12722,17 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>ADTO_DIVCT 10012022</t>
+          <t>ADTO_020122 CARTAO</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>55.00</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2022-01-10</t>
+          <t>2022-02-10</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -12779,7 +12779,7 @@
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>2022-01-10</t>
+          <t>2022-02-10</t>
         </is>
       </c>
       <c r="V66" t="inlineStr"/>
@@ -12911,17 +12911,17 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>ADTO_020122 CARTAO</t>
+          <t>ADTO_DIVCT10032022</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>200.00</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2022-02-10</t>
+          <t>2022-03-10</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -12968,7 +12968,7 @@
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>2022-02-10</t>
+          <t>2022-03-10</t>
         </is>
       </c>
       <c r="V67" t="inlineStr"/>
@@ -13100,17 +13100,17 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>ADTO_DIVCT10032022</t>
+          <t>ADTO_980948635351521</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1500.00</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-15</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -13157,7 +13157,7 @@
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-15</t>
         </is>
       </c>
       <c r="V68" t="inlineStr"/>
@@ -13289,28 +13289,28 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>ADTO_980948635351521</t>
+          <t>ADTO_06062019</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>15000.00</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2019-06-06</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>76912</t>
+          <t>77803</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr">
         <is>
-          <t>76912</t>
+          <t>77803</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -13346,7 +13346,7 @@
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2019-06-06</t>
         </is>
       </c>
       <c r="V69" t="inlineStr"/>
@@ -13478,28 +13478,28 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>ADTO_06062019</t>
+          <t>ADTO_107635A725-1</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2360.00</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2019-06-06</t>
+          <t>2021-11-30</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>77803</t>
+          <t>80551</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr">
         <is>
-          <t>77803</t>
+          <t>80551</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -13535,7 +13535,7 @@
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>2019-06-06</t>
+          <t>2021-11-30</t>
         </is>
       </c>
       <c r="V70" t="inlineStr"/>
@@ -13667,28 +13667,28 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>ADTO_107635A725-1</t>
+          <t>ADTO_29042019</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>250.00</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2021-11-30</t>
+          <t>2019-04-29</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>80551</t>
+          <t>80762</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr">
         <is>
-          <t>80551</t>
+          <t>80762</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
@@ -13724,7 +13724,7 @@
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>2021-11-30</t>
+          <t>2019-04-29</t>
         </is>
       </c>
       <c r="V71" t="inlineStr"/>
@@ -13856,28 +13856,28 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>ADTO_29042019</t>
+          <t>ADTO_FEV2020</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>7417.02</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2019-04-29</t>
+          <t>2020-02-06</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>80762</t>
+          <t>84868</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr">
         <is>
-          <t>80762</t>
+          <t>84868</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -13913,7 +13913,7 @@
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>2019-04-29</t>
+          <t>2020-02-06</t>
         </is>
       </c>
       <c r="V72" t="inlineStr"/>
@@ -14045,28 +14045,28 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>ADTO_01022022</t>
+          <t>ADTO_VIAGEM ABRIL2022</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1800.00</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>81870</t>
+          <t>86011</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr">
         <is>
-          <t>81870</t>
+          <t>86011</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -14102,7 +14102,7 @@
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="V73" t="inlineStr"/>
@@ -14234,28 +14234,28 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM MARCO2022</t>
+          <t>ADTO_141</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>40.00</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2020-10-30</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>82216</t>
+          <t>86641</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr">
         <is>
-          <t>82216</t>
+          <t>86641</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -14291,7 +14291,7 @@
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2020-10-30</t>
         </is>
       </c>
       <c r="V74" t="inlineStr"/>
@@ -14423,28 +14423,28 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>ADTO_25032022</t>
+          <t>ADTO_0081241</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2240.00</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2022-04-13</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>83495</t>
+          <t>88121</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr">
         <is>
-          <t>83495</t>
+          <t>88121</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -14480,7 +14480,7 @@
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2022-04-13</t>
         </is>
       </c>
       <c r="V75" t="inlineStr"/>
@@ -14612,28 +14612,28 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>ADTO_FEV2020</t>
+          <t>ADTO_20092021</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>62482.98</t>
+          <t>582041.25</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2020-02-06</t>
+          <t>2021-09-20</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>84868</t>
+          <t>92082</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr">
         <is>
-          <t>84868</t>
+          <t>92082</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -14669,7 +14669,7 @@
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>2020-02-06</t>
+          <t>2021-09-20</t>
         </is>
       </c>
       <c r="V76" t="inlineStr"/>
@@ -14801,28 +14801,28 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM ABRIL2022</t>
+          <t>ADTO_MAQUINA ITL50X2</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>296340.00</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2020-12-23</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>86011</t>
+          <t>92255</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
         <is>
-          <t>86011</t>
+          <t>92255</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
@@ -14858,7 +14858,7 @@
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2020-12-23</t>
         </is>
       </c>
       <c r="V77" t="inlineStr"/>
@@ -14990,28 +14990,28 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>ADTO_141</t>
+          <t>ADTO_18032021</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>197560.00</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2020-10-30</t>
+          <t>2021-03-18</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>86641</t>
+          <t>92255</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr">
         <is>
-          <t>86641</t>
+          <t>92255</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
@@ -15047,7 +15047,7 @@
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>2020-10-30</t>
+          <t>2021-03-18</t>
         </is>
       </c>
       <c r="V78" t="inlineStr"/>
@@ -15179,28 +15179,28 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>ADTO_20092021</t>
+          <t>ADTO_01062021</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>246950.00</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2021-09-20</t>
+          <t>2021-06-01</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>92082</t>
+          <t>92255</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr">
         <is>
-          <t>92082</t>
+          <t>92255</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
@@ -15236,7 +15236,7 @@
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>2021-09-20</t>
+          <t>2021-06-01</t>
         </is>
       </c>
       <c r="V79" t="inlineStr"/>
@@ -15368,17 +15368,17 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>ADTO_MAQUINA ITL50X2</t>
+          <t>ADTO_15062021</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>123475.00</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2020-12-23</t>
+          <t>2021-06-15</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -15425,7 +15425,7 @@
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>2020-12-23</t>
+          <t>2021-06-15</t>
         </is>
       </c>
       <c r="V80" t="inlineStr"/>
@@ -15557,17 +15557,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>ADTO_18032021</t>
+          <t>ADTO_15062021</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>18101.39</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2021-03-18</t>
+          <t>2021-06-15</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -15614,7 +15614,7 @@
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>2021-03-18</t>
+          <t>2021-06-15</t>
         </is>
       </c>
       <c r="V81" t="inlineStr"/>
@@ -15746,17 +15746,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>ADTO_01062021</t>
+          <t>ADTO_15072021</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>123475.00</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2021-06-01</t>
+          <t>2021-07-15</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -15803,7 +15803,7 @@
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>2021-06-01</t>
+          <t>2021-07-15</t>
         </is>
       </c>
       <c r="V82" t="inlineStr"/>
@@ -15935,17 +15935,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>ADTO_15062021</t>
+          <t>ADTO_FINAMEITAU15.07</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>48999.87</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2021-06-15</t>
+          <t>2021-07-15</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -15992,7 +15992,7 @@
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>2021-06-15</t>
+          <t>2021-07-15</t>
         </is>
       </c>
       <c r="V83" t="inlineStr"/>
@@ -16124,17 +16124,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>ADTO_15062021</t>
+          <t>ADTO_FINAMEITAU 16.08</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>49059.96</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2021-06-15</t>
+          <t>2021-08-16</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -16181,7 +16181,7 @@
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>2021-06-15</t>
+          <t>2021-08-16</t>
         </is>
       </c>
       <c r="V84" t="inlineStr"/>
@@ -16313,17 +16313,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>ADTO_15072021</t>
+          <t>ADTO_FINAMEITAU 15.09</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>48755.89</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2021-07-15</t>
+          <t>2021-09-15</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -16370,7 +16370,7 @@
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>2021-07-15</t>
+          <t>2021-09-15</t>
         </is>
       </c>
       <c r="V85" t="inlineStr"/>
@@ -16502,17 +16502,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>ADTO_FINAMEITAU15.07</t>
+          <t>ADTO_FINAMEITAU 15.10</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>48865.42</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2021-07-15</t>
+          <t>2021-10-15</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -16559,7 +16559,7 @@
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>2021-07-15</t>
+          <t>2021-10-15</t>
         </is>
       </c>
       <c r="V86" t="inlineStr"/>
@@ -16691,17 +16691,17 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>ADTO_FINAMEITAU 16.08</t>
+          <t>ADTO_12112021</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1185360.00</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2021-08-16</t>
+          <t>2021-11-12</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -16748,7 +16748,7 @@
       </c>
       <c r="U87" t="inlineStr">
         <is>
-          <t>2021-08-16</t>
+          <t>2021-11-12</t>
         </is>
       </c>
       <c r="V87" t="inlineStr"/>
@@ -16880,17 +16880,17 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>ADTO_FINAMEITAU 15.09</t>
+          <t>ADTO_FINAME</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>48627.30</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2021-09-15</t>
+          <t>2021-11-16</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -16937,7 +16937,7 @@
       </c>
       <c r="U88" t="inlineStr">
         <is>
-          <t>2021-09-15</t>
+          <t>2021-11-16</t>
         </is>
       </c>
       <c r="V88" t="inlineStr"/>
@@ -17069,17 +17069,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>ADTO_FINAMEITAU 15.10</t>
+          <t>ADTO_FINAME</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>49191.40</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2021-10-15</t>
+          <t>2021-12-15</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -17126,7 +17126,7 @@
       </c>
       <c r="U89" t="inlineStr">
         <is>
-          <t>2021-10-15</t>
+          <t>2021-12-15</t>
         </is>
       </c>
       <c r="V89" t="inlineStr"/>
@@ -17258,17 +17258,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>ADTO_12112021</t>
+          <t>ADTO_FINAME</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>354127.78</t>
+          <t>50202.75</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2021-11-12</t>
+          <t>2022-01-17</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -17315,7 +17315,7 @@
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>2021-11-12</t>
+          <t>2022-01-17</t>
         </is>
       </c>
       <c r="V90" t="inlineStr"/>
@@ -17447,17 +17447,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>ADTO_FINAME</t>
+          <t>ADTO_FINAME 15022022</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>49720.00</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2021-11-16</t>
+          <t>2022-02-15</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -17504,7 +17504,7 @@
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>2021-11-16</t>
+          <t>2022-02-15</t>
         </is>
       </c>
       <c r="V91" t="inlineStr"/>
@@ -17636,17 +17636,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>ADTO_FINAME</t>
+          <t>ADTO_FINAME 15032022</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>48865.53</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2021-12-15</t>
+          <t>2022-03-15</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -17693,7 +17693,7 @@
       </c>
       <c r="U92" t="inlineStr">
         <is>
-          <t>2021-12-15</t>
+          <t>2022-03-15</t>
         </is>
       </c>
       <c r="V92" t="inlineStr"/>
@@ -17825,28 +17825,28 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>ADTO_FINAME</t>
+          <t>ADTO_08042022</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>690.00</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2022-01-17</t>
+          <t>2022-04-08</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>92255</t>
+          <t>96259</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
-          <t>92255</t>
+          <t>96259</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -17882,7 +17882,7 @@
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>2022-01-17</t>
+          <t>2022-04-08</t>
         </is>
       </c>
       <c r="V93" t="inlineStr"/>
@@ -18014,28 +18014,28 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>ADTO_FINAME 15022022</t>
+          <t>ADTO_PINTURAS</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2022-02-15</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>92255</t>
+          <t>98796</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr">
         <is>
-          <t>92255</t>
+          <t>98796</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -18071,7 +18071,7 @@
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>2022-02-15</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="V94" t="inlineStr"/>
@@ -18203,28 +18203,28 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>ADTO_FINAME 15032022</t>
+          <t>ADTO_36586COMPL.</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>375.64</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2021-11-30</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>92255</t>
+          <t>99472</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr">
         <is>
-          <t>92255</t>
+          <t>99472</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -18260,7 +18260,7 @@
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2021-11-30</t>
         </is>
       </c>
       <c r="V95" t="inlineStr"/>
@@ -18392,28 +18392,28 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>ADTO_CTES 25-11-2021</t>
+          <t>ADTO_VIAGEM MARCO2022</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1000.00</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2021-11-29</t>
+          <t>2022-03-08</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>98431</t>
+          <t>99818</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr">
         <is>
-          <t>98431</t>
+          <t>99818</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -18449,7 +18449,7 @@
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>2021-11-29</t>
+          <t>2022-03-08</t>
         </is>
       </c>
       <c r="V96" t="inlineStr"/>
@@ -18581,28 +18581,28 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>ADTO_415</t>
+          <t>ADTO_1648815709</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2003.00</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2022-02-22</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>98431</t>
+          <t>100361</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
       <c r="I97" t="inlineStr">
         <is>
-          <t>98431</t>
+          <t>100361</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -18638,7 +18638,7 @@
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>2022-02-22</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="V97" t="inlineStr"/>
@@ -18770,28 +18770,28 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>ADTO_PINTURAS</t>
+          <t>ADTO_1648815457</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>5253.00</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2021-10-06</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>98796</t>
+          <t>100361</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr">
         <is>
-          <t>98796</t>
+          <t>100361</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -18827,7 +18827,7 @@
       </c>
       <c r="U98" t="inlineStr">
         <is>
-          <t>2021-10-06</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="V98" t="inlineStr"/>
@@ -18959,28 +18959,28 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>ADTO_36586COMPL.</t>
+          <t>ADTO_1649187040</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1198.00</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2021-11-30</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>99472</t>
+          <t>100361</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr">
         <is>
-          <t>99472</t>
+          <t>100361</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -19016,7 +19016,7 @@
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>2021-11-30</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="V99" t="inlineStr"/>
@@ -19148,28 +19148,28 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM MARCO2022</t>
+          <t>ADTO_VIAGEM ABRIL2022</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>3000.00</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2022-03-08</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>99818</t>
+          <t>103177</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr">
         <is>
-          <t>99818</t>
+          <t>103177</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -19205,7 +19205,7 @@
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>2022-03-08</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="V100" t="inlineStr"/>
@@ -19337,28 +19337,28 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM MARCO22</t>
+          <t>ADTO_VIAGEM ABRIL2022</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2000.00</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2022-02-22</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>103175</t>
+          <t>103182</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
       <c r="I101" t="inlineStr">
         <is>
-          <t>103175</t>
+          <t>103182</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
@@ -19394,7 +19394,7 @@
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>2022-02-22</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="V101" t="inlineStr"/>
@@ -19526,28 +19526,28 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM MARCO2022</t>
+          <t>ADTO_VIAGEM ABRIL2022</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1400.00</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2022-03-22</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>103175</t>
+          <t>103236</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
       <c r="I102" t="inlineStr">
         <is>
-          <t>103175</t>
+          <t>103236</t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
@@ -19583,7 +19583,7 @@
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>2022-03-22</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="V102" t="inlineStr"/>
@@ -19720,23 +19720,23 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1400.00</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>103177</t>
+          <t>103244</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
       <c r="I103" t="inlineStr">
         <is>
-          <t>103177</t>
+          <t>103244</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
@@ -19772,7 +19772,7 @@
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="V103" t="inlineStr"/>
@@ -19904,28 +19904,28 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM ABRIL2022</t>
+          <t>ADTO_VIAGEM MARCO2022</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1300.00</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2022-03-07</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>103182</t>
+          <t>103334</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr">
         <is>
-          <t>103182</t>
+          <t>103334</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
@@ -19961,7 +19961,7 @@
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2022-03-07</t>
         </is>
       </c>
       <c r="V104" t="inlineStr"/>
@@ -20098,23 +20098,23 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>150.00</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2022-03-17</t>
+          <t>2022-03-25</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>103215</t>
+          <t>104176</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr">
         <is>
-          <t>103215</t>
+          <t>104176</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
@@ -20150,7 +20150,7 @@
       </c>
       <c r="U105" t="inlineStr">
         <is>
-          <t>2022-03-17</t>
+          <t>2022-03-25</t>
         </is>
       </c>
       <c r="V105" t="inlineStr"/>
@@ -20287,23 +20287,23 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>700.00</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>103236</t>
+          <t>104176</t>
         </is>
       </c>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr">
         <is>
-          <t>103236</t>
+          <t>104176</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -20339,7 +20339,7 @@
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="V106" t="inlineStr"/>
@@ -20471,28 +20471,28 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM ABRIL2022</t>
+          <t>ADTO_NF 8137</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>5535.00</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2022-03-22</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>103244</t>
+          <t>104485</t>
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr">
         <is>
-          <t>103244</t>
+          <t>104485</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
@@ -20528,7 +20528,7 @@
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>2022-03-30</t>
+          <t>2022-03-22</t>
         </is>
       </c>
       <c r="V107" t="inlineStr"/>
@@ -20665,23 +20665,23 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1300.00</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2022-03-22</t>
+          <t>2022-03-24</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>103311</t>
+          <t>104606</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr">
         <is>
-          <t>103311</t>
+          <t>104606</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
@@ -20717,7 +20717,7 @@
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>2022-03-22</t>
+          <t>2022-03-24</t>
         </is>
       </c>
       <c r="V108" t="inlineStr"/>
@@ -20849,28 +20849,28 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>ADTO_VIAGEM MARCO2022</t>
+          <t>ADTO_PC 15486.V2</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>189.13</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2022-03-07</t>
+          <t>2022-04-04</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>103334</t>
+          <t>104805</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr">
         <is>
-          <t>103334</t>
+          <t>104805</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
@@ -20906,7 +20906,7 @@
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>2022-03-07</t>
+          <t>2022-04-04</t>
         </is>
       </c>
       <c r="V109" t="inlineStr"/>
@@ -21038,28 +21038,28 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>ADTO_PV 26931</t>
+          <t>ADTO_04042022</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>15000.00</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>2022-02-24</t>
+          <t>2022-04-04</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>103885</t>
+          <t>104816</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
       <c r="I110" t="inlineStr">
         <is>
-          <t>103885</t>
+          <t>104816</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
@@ -21095,7 +21095,7 @@
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>2022-02-24</t>
+          <t>2022-04-04</t>
         </is>
       </c>
       <c r="V110" t="inlineStr"/>
@@ -21211,762 +21211,6 @@
         </is>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>111</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>CEDISA_BU</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>CARGA</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>ADTO_VIAGEM MARCO2022</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>2022-03-25</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>104176</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>104176</t>
-        </is>
-      </c>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="L111" t="inlineStr">
-        <is>
-          <t>CARGA DE SALDOS - ADIANTAMENTOS</t>
-        </is>
-      </c>
-      <c r="M111" t="inlineStr"/>
-      <c r="N111" t="inlineStr">
-        <is>
-          <t>PREPAYMENT</t>
-        </is>
-      </c>
-      <c r="O111" t="inlineStr"/>
-      <c r="P111" t="inlineStr"/>
-      <c r="Q111" t="inlineStr"/>
-      <c r="R111" t="inlineStr"/>
-      <c r="S111" t="inlineStr"/>
-      <c r="T111" t="inlineStr">
-        <is>
-          <t>IMEDIATO</t>
-        </is>
-      </c>
-      <c r="U111" t="inlineStr">
-        <is>
-          <t>2022-03-25</t>
-        </is>
-      </c>
-      <c r="V111" t="inlineStr"/>
-      <c r="W111" t="inlineStr"/>
-      <c r="X111" t="inlineStr">
-        <is>
-          <t>2022/03/29</t>
-        </is>
-      </c>
-      <c r="Y111" t="inlineStr">
-        <is>
-          <t>BR_BAIXA_MANUAL</t>
-        </is>
-      </c>
-      <c r="Z111" t="inlineStr">
-        <is>
-          <t>ADIANTAMENTO</t>
-        </is>
-      </c>
-      <c r="AA111" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AB111" t="inlineStr"/>
-      <c r="AC111" t="inlineStr"/>
-      <c r="AD111" t="inlineStr"/>
-      <c r="AE111" t="inlineStr"/>
-      <c r="AF111" t="inlineStr"/>
-      <c r="AG111" t="inlineStr"/>
-      <c r="AH111" t="inlineStr"/>
-      <c r="AI111" t="inlineStr"/>
-      <c r="AJ111" t="inlineStr"/>
-      <c r="AK111" t="inlineStr">
-        <is>
-          <t>1001.000.000.21110001.0000.0000.0.0</t>
-        </is>
-      </c>
-      <c r="AL111" t="inlineStr"/>
-      <c r="AM111" t="inlineStr"/>
-      <c r="AN111" t="inlineStr"/>
-      <c r="AO111" t="inlineStr"/>
-      <c r="AP111" t="inlineStr"/>
-      <c r="AQ111" t="inlineStr"/>
-      <c r="AR111" t="inlineStr"/>
-      <c r="AS111" t="inlineStr"/>
-      <c r="AT111" t="inlineStr"/>
-      <c r="AU111" t="inlineStr"/>
-      <c r="AV111" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AW111" t="inlineStr"/>
-      <c r="AX111" t="inlineStr"/>
-      <c r="AY111" t="inlineStr"/>
-      <c r="AZ111" t="inlineStr"/>
-      <c r="BA111" t="inlineStr"/>
-      <c r="BB111" t="inlineStr"/>
-      <c r="BC111" t="inlineStr"/>
-      <c r="BD111" t="inlineStr"/>
-      <c r="BE111" t="inlineStr"/>
-      <c r="BF111" t="inlineStr"/>
-      <c r="BG111" t="inlineStr"/>
-      <c r="BH111" t="inlineStr"/>
-      <c r="BI111" t="inlineStr"/>
-      <c r="BJ111" t="inlineStr"/>
-      <c r="BK111" t="inlineStr"/>
-      <c r="BL111" t="inlineStr"/>
-      <c r="BM111" t="inlineStr"/>
-      <c r="BN111" t="inlineStr"/>
-      <c r="BO111" t="inlineStr"/>
-      <c r="BP111" t="inlineStr"/>
-      <c r="BQ111" t="inlineStr"/>
-      <c r="BR111" t="inlineStr"/>
-      <c r="BS111" t="inlineStr"/>
-      <c r="BT111" t="inlineStr"/>
-      <c r="BU111" t="inlineStr"/>
-      <c r="BV111" t="inlineStr"/>
-      <c r="BW111" t="inlineStr"/>
-      <c r="BX111" t="inlineStr"/>
-      <c r="BY111" t="inlineStr"/>
-      <c r="BZ111" t="inlineStr"/>
-      <c r="CA111" t="inlineStr"/>
-      <c r="CB111" t="inlineStr"/>
-      <c r="CC111" t="inlineStr"/>
-      <c r="CD111" t="inlineStr"/>
-      <c r="CE111" t="inlineStr"/>
-      <c r="CF111" t="inlineStr"/>
-      <c r="CG111" t="inlineStr"/>
-      <c r="CH111" t="inlineStr"/>
-      <c r="CI111" t="inlineStr"/>
-      <c r="CJ111" t="inlineStr"/>
-      <c r="CK111" t="inlineStr"/>
-      <c r="CL111" t="inlineStr"/>
-      <c r="CM111" t="inlineStr"/>
-      <c r="CN111" t="inlineStr"/>
-      <c r="CO111" t="inlineStr"/>
-      <c r="CP111" t="inlineStr"/>
-      <c r="CQ111" t="inlineStr"/>
-      <c r="CR111" t="inlineStr"/>
-      <c r="CS111" t="inlineStr"/>
-      <c r="CT111" t="inlineStr"/>
-      <c r="CU111" t="inlineStr"/>
-      <c r="CV111" t="inlineStr">
-        <is>
-          <t>JL_BR_APXINWKB_AP_INVOICES</t>
-        </is>
-      </c>
-      <c r="CW111" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>112</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>CEDISA_BU</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>CARGA</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>ADTO_VIAGEM ABRIL2022</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>2022-03-28</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>104176</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr"/>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>104176</t>
-        </is>
-      </c>
-      <c r="J112" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>CARGA DE SALDOS - ADIANTAMENTOS</t>
-        </is>
-      </c>
-      <c r="M112" t="inlineStr"/>
-      <c r="N112" t="inlineStr">
-        <is>
-          <t>PREPAYMENT</t>
-        </is>
-      </c>
-      <c r="O112" t="inlineStr"/>
-      <c r="P112" t="inlineStr"/>
-      <c r="Q112" t="inlineStr"/>
-      <c r="R112" t="inlineStr"/>
-      <c r="S112" t="inlineStr"/>
-      <c r="T112" t="inlineStr">
-        <is>
-          <t>IMEDIATO</t>
-        </is>
-      </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>2022-03-28</t>
-        </is>
-      </c>
-      <c r="V112" t="inlineStr"/>
-      <c r="W112" t="inlineStr"/>
-      <c r="X112" t="inlineStr">
-        <is>
-          <t>2022/03/29</t>
-        </is>
-      </c>
-      <c r="Y112" t="inlineStr">
-        <is>
-          <t>BR_BAIXA_MANUAL</t>
-        </is>
-      </c>
-      <c r="Z112" t="inlineStr">
-        <is>
-          <t>ADIANTAMENTO</t>
-        </is>
-      </c>
-      <c r="AA112" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AB112" t="inlineStr"/>
-      <c r="AC112" t="inlineStr"/>
-      <c r="AD112" t="inlineStr"/>
-      <c r="AE112" t="inlineStr"/>
-      <c r="AF112" t="inlineStr"/>
-      <c r="AG112" t="inlineStr"/>
-      <c r="AH112" t="inlineStr"/>
-      <c r="AI112" t="inlineStr"/>
-      <c r="AJ112" t="inlineStr"/>
-      <c r="AK112" t="inlineStr">
-        <is>
-          <t>1001.000.000.21110001.0000.0000.0.0</t>
-        </is>
-      </c>
-      <c r="AL112" t="inlineStr"/>
-      <c r="AM112" t="inlineStr"/>
-      <c r="AN112" t="inlineStr"/>
-      <c r="AO112" t="inlineStr"/>
-      <c r="AP112" t="inlineStr"/>
-      <c r="AQ112" t="inlineStr"/>
-      <c r="AR112" t="inlineStr"/>
-      <c r="AS112" t="inlineStr"/>
-      <c r="AT112" t="inlineStr"/>
-      <c r="AU112" t="inlineStr"/>
-      <c r="AV112" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AW112" t="inlineStr"/>
-      <c r="AX112" t="inlineStr"/>
-      <c r="AY112" t="inlineStr"/>
-      <c r="AZ112" t="inlineStr"/>
-      <c r="BA112" t="inlineStr"/>
-      <c r="BB112" t="inlineStr"/>
-      <c r="BC112" t="inlineStr"/>
-      <c r="BD112" t="inlineStr"/>
-      <c r="BE112" t="inlineStr"/>
-      <c r="BF112" t="inlineStr"/>
-      <c r="BG112" t="inlineStr"/>
-      <c r="BH112" t="inlineStr"/>
-      <c r="BI112" t="inlineStr"/>
-      <c r="BJ112" t="inlineStr"/>
-      <c r="BK112" t="inlineStr"/>
-      <c r="BL112" t="inlineStr"/>
-      <c r="BM112" t="inlineStr"/>
-      <c r="BN112" t="inlineStr"/>
-      <c r="BO112" t="inlineStr"/>
-      <c r="BP112" t="inlineStr"/>
-      <c r="BQ112" t="inlineStr"/>
-      <c r="BR112" t="inlineStr"/>
-      <c r="BS112" t="inlineStr"/>
-      <c r="BT112" t="inlineStr"/>
-      <c r="BU112" t="inlineStr"/>
-      <c r="BV112" t="inlineStr"/>
-      <c r="BW112" t="inlineStr"/>
-      <c r="BX112" t="inlineStr"/>
-      <c r="BY112" t="inlineStr"/>
-      <c r="BZ112" t="inlineStr"/>
-      <c r="CA112" t="inlineStr"/>
-      <c r="CB112" t="inlineStr"/>
-      <c r="CC112" t="inlineStr"/>
-      <c r="CD112" t="inlineStr"/>
-      <c r="CE112" t="inlineStr"/>
-      <c r="CF112" t="inlineStr"/>
-      <c r="CG112" t="inlineStr"/>
-      <c r="CH112" t="inlineStr"/>
-      <c r="CI112" t="inlineStr"/>
-      <c r="CJ112" t="inlineStr"/>
-      <c r="CK112" t="inlineStr"/>
-      <c r="CL112" t="inlineStr"/>
-      <c r="CM112" t="inlineStr"/>
-      <c r="CN112" t="inlineStr"/>
-      <c r="CO112" t="inlineStr"/>
-      <c r="CP112" t="inlineStr"/>
-      <c r="CQ112" t="inlineStr"/>
-      <c r="CR112" t="inlineStr"/>
-      <c r="CS112" t="inlineStr"/>
-      <c r="CT112" t="inlineStr"/>
-      <c r="CU112" t="inlineStr"/>
-      <c r="CV112" t="inlineStr">
-        <is>
-          <t>JL_BR_APXINWKB_AP_INVOICES</t>
-        </is>
-      </c>
-      <c r="CW112" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>113</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>CEDISA_BU</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>CARGA</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>ADTO_NF 8137</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>2022-03-22</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>104485</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr"/>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>104485</t>
-        </is>
-      </c>
-      <c r="J113" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>CARGA DE SALDOS - ADIANTAMENTOS</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr"/>
-      <c r="N113" t="inlineStr">
-        <is>
-          <t>PREPAYMENT</t>
-        </is>
-      </c>
-      <c r="O113" t="inlineStr"/>
-      <c r="P113" t="inlineStr"/>
-      <c r="Q113" t="inlineStr"/>
-      <c r="R113" t="inlineStr"/>
-      <c r="S113" t="inlineStr"/>
-      <c r="T113" t="inlineStr">
-        <is>
-          <t>IMEDIATO</t>
-        </is>
-      </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>2022-03-22</t>
-        </is>
-      </c>
-      <c r="V113" t="inlineStr"/>
-      <c r="W113" t="inlineStr"/>
-      <c r="X113" t="inlineStr">
-        <is>
-          <t>2022/03/29</t>
-        </is>
-      </c>
-      <c r="Y113" t="inlineStr">
-        <is>
-          <t>BR_BAIXA_MANUAL</t>
-        </is>
-      </c>
-      <c r="Z113" t="inlineStr">
-        <is>
-          <t>ADIANTAMENTO</t>
-        </is>
-      </c>
-      <c r="AA113" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AB113" t="inlineStr"/>
-      <c r="AC113" t="inlineStr"/>
-      <c r="AD113" t="inlineStr"/>
-      <c r="AE113" t="inlineStr"/>
-      <c r="AF113" t="inlineStr"/>
-      <c r="AG113" t="inlineStr"/>
-      <c r="AH113" t="inlineStr"/>
-      <c r="AI113" t="inlineStr"/>
-      <c r="AJ113" t="inlineStr"/>
-      <c r="AK113" t="inlineStr">
-        <is>
-          <t>1001.000.000.21110001.0000.0000.0.0</t>
-        </is>
-      </c>
-      <c r="AL113" t="inlineStr"/>
-      <c r="AM113" t="inlineStr"/>
-      <c r="AN113" t="inlineStr"/>
-      <c r="AO113" t="inlineStr"/>
-      <c r="AP113" t="inlineStr"/>
-      <c r="AQ113" t="inlineStr"/>
-      <c r="AR113" t="inlineStr"/>
-      <c r="AS113" t="inlineStr"/>
-      <c r="AT113" t="inlineStr"/>
-      <c r="AU113" t="inlineStr"/>
-      <c r="AV113" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AW113" t="inlineStr"/>
-      <c r="AX113" t="inlineStr"/>
-      <c r="AY113" t="inlineStr"/>
-      <c r="AZ113" t="inlineStr"/>
-      <c r="BA113" t="inlineStr"/>
-      <c r="BB113" t="inlineStr"/>
-      <c r="BC113" t="inlineStr"/>
-      <c r="BD113" t="inlineStr"/>
-      <c r="BE113" t="inlineStr"/>
-      <c r="BF113" t="inlineStr"/>
-      <c r="BG113" t="inlineStr"/>
-      <c r="BH113" t="inlineStr"/>
-      <c r="BI113" t="inlineStr"/>
-      <c r="BJ113" t="inlineStr"/>
-      <c r="BK113" t="inlineStr"/>
-      <c r="BL113" t="inlineStr"/>
-      <c r="BM113" t="inlineStr"/>
-      <c r="BN113" t="inlineStr"/>
-      <c r="BO113" t="inlineStr"/>
-      <c r="BP113" t="inlineStr"/>
-      <c r="BQ113" t="inlineStr"/>
-      <c r="BR113" t="inlineStr"/>
-      <c r="BS113" t="inlineStr"/>
-      <c r="BT113" t="inlineStr"/>
-      <c r="BU113" t="inlineStr"/>
-      <c r="BV113" t="inlineStr"/>
-      <c r="BW113" t="inlineStr"/>
-      <c r="BX113" t="inlineStr"/>
-      <c r="BY113" t="inlineStr"/>
-      <c r="BZ113" t="inlineStr"/>
-      <c r="CA113" t="inlineStr"/>
-      <c r="CB113" t="inlineStr"/>
-      <c r="CC113" t="inlineStr"/>
-      <c r="CD113" t="inlineStr"/>
-      <c r="CE113" t="inlineStr"/>
-      <c r="CF113" t="inlineStr"/>
-      <c r="CG113" t="inlineStr"/>
-      <c r="CH113" t="inlineStr"/>
-      <c r="CI113" t="inlineStr"/>
-      <c r="CJ113" t="inlineStr"/>
-      <c r="CK113" t="inlineStr"/>
-      <c r="CL113" t="inlineStr"/>
-      <c r="CM113" t="inlineStr"/>
-      <c r="CN113" t="inlineStr"/>
-      <c r="CO113" t="inlineStr"/>
-      <c r="CP113" t="inlineStr"/>
-      <c r="CQ113" t="inlineStr"/>
-      <c r="CR113" t="inlineStr"/>
-      <c r="CS113" t="inlineStr"/>
-      <c r="CT113" t="inlineStr"/>
-      <c r="CU113" t="inlineStr"/>
-      <c r="CV113" t="inlineStr">
-        <is>
-          <t>JL_BR_APXINWKB_AP_INVOICES</t>
-        </is>
-      </c>
-      <c r="CW113" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>114</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>CEDISA_BU</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>CARGA</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>ADTO_VIAGEM MARCO2022</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>2022-03-24</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>104606</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr"/>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>104606</t>
-        </is>
-      </c>
-      <c r="J114" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>BRL</t>
-        </is>
-      </c>
-      <c r="L114" t="inlineStr">
-        <is>
-          <t>CARGA DE SALDOS - ADIANTAMENTOS</t>
-        </is>
-      </c>
-      <c r="M114" t="inlineStr"/>
-      <c r="N114" t="inlineStr">
-        <is>
-          <t>PREPAYMENT</t>
-        </is>
-      </c>
-      <c r="O114" t="inlineStr"/>
-      <c r="P114" t="inlineStr"/>
-      <c r="Q114" t="inlineStr"/>
-      <c r="R114" t="inlineStr"/>
-      <c r="S114" t="inlineStr"/>
-      <c r="T114" t="inlineStr">
-        <is>
-          <t>IMEDIATO</t>
-        </is>
-      </c>
-      <c r="U114" t="inlineStr">
-        <is>
-          <t>2022-03-24</t>
-        </is>
-      </c>
-      <c r="V114" t="inlineStr"/>
-      <c r="W114" t="inlineStr"/>
-      <c r="X114" t="inlineStr">
-        <is>
-          <t>2022/03/29</t>
-        </is>
-      </c>
-      <c r="Y114" t="inlineStr">
-        <is>
-          <t>BR_BAIXA_MANUAL</t>
-        </is>
-      </c>
-      <c r="Z114" t="inlineStr">
-        <is>
-          <t>ADIANTAMENTO</t>
-        </is>
-      </c>
-      <c r="AA114" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AB114" t="inlineStr"/>
-      <c r="AC114" t="inlineStr"/>
-      <c r="AD114" t="inlineStr"/>
-      <c r="AE114" t="inlineStr"/>
-      <c r="AF114" t="inlineStr"/>
-      <c r="AG114" t="inlineStr"/>
-      <c r="AH114" t="inlineStr"/>
-      <c r="AI114" t="inlineStr"/>
-      <c r="AJ114" t="inlineStr"/>
-      <c r="AK114" t="inlineStr">
-        <is>
-          <t>1001.000.000.21110001.0000.0000.0.0</t>
-        </is>
-      </c>
-      <c r="AL114" t="inlineStr"/>
-      <c r="AM114" t="inlineStr"/>
-      <c r="AN114" t="inlineStr"/>
-      <c r="AO114" t="inlineStr"/>
-      <c r="AP114" t="inlineStr"/>
-      <c r="AQ114" t="inlineStr"/>
-      <c r="AR114" t="inlineStr"/>
-      <c r="AS114" t="inlineStr"/>
-      <c r="AT114" t="inlineStr"/>
-      <c r="AU114" t="inlineStr"/>
-      <c r="AV114" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AW114" t="inlineStr"/>
-      <c r="AX114" t="inlineStr"/>
-      <c r="AY114" t="inlineStr"/>
-      <c r="AZ114" t="inlineStr"/>
-      <c r="BA114" t="inlineStr"/>
-      <c r="BB114" t="inlineStr"/>
-      <c r="BC114" t="inlineStr"/>
-      <c r="BD114" t="inlineStr"/>
-      <c r="BE114" t="inlineStr"/>
-      <c r="BF114" t="inlineStr"/>
-      <c r="BG114" t="inlineStr"/>
-      <c r="BH114" t="inlineStr"/>
-      <c r="BI114" t="inlineStr"/>
-      <c r="BJ114" t="inlineStr"/>
-      <c r="BK114" t="inlineStr"/>
-      <c r="BL114" t="inlineStr"/>
-      <c r="BM114" t="inlineStr"/>
-      <c r="BN114" t="inlineStr"/>
-      <c r="BO114" t="inlineStr"/>
-      <c r="BP114" t="inlineStr"/>
-      <c r="BQ114" t="inlineStr"/>
-      <c r="BR114" t="inlineStr"/>
-      <c r="BS114" t="inlineStr"/>
-      <c r="BT114" t="inlineStr"/>
-      <c r="BU114" t="inlineStr"/>
-      <c r="BV114" t="inlineStr"/>
-      <c r="BW114" t="inlineStr"/>
-      <c r="BX114" t="inlineStr"/>
-      <c r="BY114" t="inlineStr"/>
-      <c r="BZ114" t="inlineStr"/>
-      <c r="CA114" t="inlineStr"/>
-      <c r="CB114" t="inlineStr"/>
-      <c r="CC114" t="inlineStr"/>
-      <c r="CD114" t="inlineStr"/>
-      <c r="CE114" t="inlineStr"/>
-      <c r="CF114" t="inlineStr"/>
-      <c r="CG114" t="inlineStr"/>
-      <c r="CH114" t="inlineStr"/>
-      <c r="CI114" t="inlineStr"/>
-      <c r="CJ114" t="inlineStr"/>
-      <c r="CK114" t="inlineStr"/>
-      <c r="CL114" t="inlineStr"/>
-      <c r="CM114" t="inlineStr"/>
-      <c r="CN114" t="inlineStr"/>
-      <c r="CO114" t="inlineStr"/>
-      <c r="CP114" t="inlineStr"/>
-      <c r="CQ114" t="inlineStr"/>
-      <c r="CR114" t="inlineStr"/>
-      <c r="CS114" t="inlineStr"/>
-      <c r="CT114" t="inlineStr"/>
-      <c r="CU114" t="inlineStr"/>
-      <c r="CV114" t="inlineStr">
-        <is>
-          <t>JL_BR_APXINWKB_AP_INVOICES</t>
-        </is>
-      </c>
-      <c r="CW114" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>